<commit_message>
blocked customer table added
</commit_message>
<xml_diff>
--- a/Database/Database_schema.xlsx
+++ b/Database/Database_schema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tatvasoft_training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tatvasoft_training\training_project\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACD36FA-DB96-465B-A8B0-6FECDE22D9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07516DB1-5418-479E-8E7B-01922504C693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{22156182-C924-4F72-AF67-E5D9D3BCE709}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="126">
   <si>
     <t>Description : for storing emails of get our news letter</t>
   </si>
@@ -392,6 +392,24 @@
   </si>
   <si>
     <t>feedback</t>
+  </si>
+  <si>
+    <t>sp_blocked_customer</t>
+  </si>
+  <si>
+    <t>Description : for storing blocked customer ID of particular service provider</t>
+  </si>
+  <si>
+    <t>spb_c_id</t>
+  </si>
+  <si>
+    <t>blocked_c_id</t>
+  </si>
+  <si>
+    <t>service_active_status</t>
+  </si>
+  <si>
+    <t>for active:true ,completed/cancelled :false</t>
   </si>
 </sst>
 </file>
@@ -447,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -458,7 +476,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -775,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA62D68-321F-4B17-BCFF-253E0FD943A8}">
-  <dimension ref="A1:E168"/>
+  <dimension ref="A1:E177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="D168" sqref="D168"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="E142" sqref="E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -792,29 +816,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
@@ -865,29 +889,29 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
@@ -980,29 +1004,29 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
@@ -1075,29 +1099,29 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
@@ -1148,29 +1172,29 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
@@ -1302,29 +1326,29 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
     </row>
     <row r="53" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
@@ -1372,29 +1396,29 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
@@ -1484,29 +1508,29 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
@@ -1551,29 +1575,29 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
@@ -1614,33 +1638,33 @@
         <v>7</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
@@ -1870,29 +1894,29 @@
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A108" s="4" t="s">
+      <c r="A108" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B108" s="4"/>
-      <c r="C108" s="4"/>
-      <c r="D108" s="4"/>
-      <c r="E108" s="4"/>
+      <c r="B108" s="5"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A109" s="4"/>
-      <c r="B109" s="4"/>
-      <c r="C109" s="4"/>
-      <c r="D109" s="4"/>
-      <c r="E109" s="4"/>
+      <c r="A109" s="5"/>
+      <c r="B109" s="5"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A110" s="2" t="s">
+      <c r="A110" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
-      <c r="D110" s="2"/>
-      <c r="E110" s="2"/>
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
@@ -1943,29 +1967,29 @@
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A116" s="4" t="s">
+      <c r="A116" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B116" s="4"/>
-      <c r="C116" s="4"/>
-      <c r="D116" s="4"/>
-      <c r="E116" s="4"/>
+      <c r="B116" s="5"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A117" s="4"/>
-      <c r="B117" s="4"/>
-      <c r="C117" s="4"/>
-      <c r="D117" s="4"/>
-      <c r="E117" s="4"/>
+      <c r="A117" s="5"/>
+      <c r="B117" s="5"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A118" s="2" t="s">
+      <c r="A118" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
-      <c r="D118" s="2"/>
-      <c r="E118" s="2"/>
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
@@ -2066,29 +2090,29 @@
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A128" s="4" t="s">
+      <c r="A128" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B128" s="4"/>
-      <c r="C128" s="4"/>
-      <c r="D128" s="4"/>
-      <c r="E128" s="4"/>
+      <c r="B128" s="5"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="5"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A129" s="4"/>
-      <c r="B129" s="4"/>
-      <c r="C129" s="4"/>
-      <c r="D129" s="4"/>
-      <c r="E129" s="4"/>
+      <c r="A129" s="5"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="5"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A130" s="2" t="s">
+      <c r="A130" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B130" s="2"/>
-      <c r="C130" s="2"/>
-      <c r="D130" s="2"/>
-      <c r="E130" s="2"/>
+      <c r="B130" s="6"/>
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
+      <c r="E130" s="6"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
@@ -2230,199 +2254,199 @@
         <v>16</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A143" s="4" t="s">
+    <row r="142" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A142" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E142" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A144" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B143" s="4"/>
-      <c r="C143" s="4"/>
-      <c r="D143" s="4"/>
-      <c r="E143" s="4"/>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A144" s="4"/>
-      <c r="B144" s="4"/>
-      <c r="C144" s="4"/>
-      <c r="D144" s="4"/>
-      <c r="E144" s="4"/>
+      <c r="B144" s="5"/>
+      <c r="C144" s="5"/>
+      <c r="D144" s="5"/>
+      <c r="E144" s="5"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A145" s="2" t="s">
+      <c r="A145" s="5"/>
+      <c r="B145" s="5"/>
+      <c r="C145" s="5"/>
+      <c r="D145" s="5"/>
+      <c r="E145" s="5"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A146" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B145" s="2"/>
-      <c r="C145" s="2"/>
-      <c r="D145" s="2"/>
-      <c r="E145" s="2"/>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A147" s="3" t="s">
+      <c r="B146" s="6"/>
+      <c r="C146" s="6"/>
+      <c r="D146" s="6"/>
+      <c r="E146" s="6"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A148" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B147" s="3" t="s">
+      <c r="B148" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C147" s="3" t="s">
+      <c r="C148" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D147" s="3" t="s">
+      <c r="D148" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E147" s="3" t="s">
+      <c r="E148" s="3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A148" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A150" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A151" s="4" t="s">
+      <c r="B150" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A152" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B151" s="4"/>
-      <c r="C151" s="4"/>
-      <c r="D151" s="4"/>
-      <c r="E151" s="4"/>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A152" s="4"/>
-      <c r="B152" s="4"/>
-      <c r="C152" s="4"/>
-      <c r="D152" s="4"/>
-      <c r="E152" s="4"/>
+      <c r="B152" s="5"/>
+      <c r="C152" s="5"/>
+      <c r="D152" s="5"/>
+      <c r="E152" s="5"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A153" s="2" t="s">
+      <c r="A153" s="5"/>
+      <c r="B153" s="5"/>
+      <c r="C153" s="5"/>
+      <c r="D153" s="5"/>
+      <c r="E153" s="5"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A154" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B153" s="2"/>
-      <c r="C153" s="2"/>
-      <c r="D153" s="2"/>
-      <c r="E153" s="2"/>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A155" s="3" t="s">
+      <c r="B154" s="6"/>
+      <c r="C154" s="6"/>
+      <c r="D154" s="6"/>
+      <c r="E154" s="6"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A156" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B155" s="3" t="s">
+      <c r="B156" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C155" s="3" t="s">
+      <c r="C156" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D155" s="3" t="s">
+      <c r="D156" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E155" s="3" t="s">
+      <c r="E156" s="3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A156" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A158" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B157" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C157" s="1">
+      <c r="B158" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158" s="1">
         <v>70</v>
       </c>
-      <c r="D157" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A159" s="4" t="s">
+      <c r="D158" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A160" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B159" s="4"/>
-      <c r="C159" s="4"/>
-      <c r="D159" s="4"/>
-      <c r="E159" s="4"/>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A160" s="4"/>
-      <c r="B160" s="4"/>
-      <c r="C160" s="4"/>
-      <c r="D160" s="4"/>
-      <c r="E160" s="4"/>
+      <c r="B160" s="5"/>
+      <c r="C160" s="5"/>
+      <c r="D160" s="5"/>
+      <c r="E160" s="5"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A161" s="2" t="s">
+      <c r="A161" s="5"/>
+      <c r="B161" s="5"/>
+      <c r="C161" s="5"/>
+      <c r="D161" s="5"/>
+      <c r="E161" s="5"/>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A162" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B161" s="2"/>
-      <c r="C161" s="2"/>
-      <c r="D161" s="2"/>
-      <c r="E161" s="2"/>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A163" s="3" t="s">
+      <c r="B162" s="6"/>
+      <c r="C162" s="6"/>
+      <c r="D162" s="6"/>
+      <c r="E162" s="6"/>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A164" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B163" s="3" t="s">
+      <c r="B164" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C163" s="3" t="s">
+      <c r="C164" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D163" s="3" t="s">
+      <c r="D164" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E163" s="3" t="s">
+      <c r="E164" s="3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A164" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>7</v>
@@ -2431,12 +2455,12 @@
         <v>16</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>7</v>
@@ -2450,7 +2474,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>7</v>
@@ -2464,40 +2488,126 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A169" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B168" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C168" s="1">
+      <c r="B169" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C169" s="1">
         <v>100</v>
       </c>
-      <c r="D168" s="1" t="s">
+      <c r="D169" s="1" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A171" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B171" s="5"/>
+      <c r="C171" s="5"/>
+      <c r="D171" s="5"/>
+      <c r="E171" s="5"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A172" s="5"/>
+      <c r="B172" s="5"/>
+      <c r="C172" s="5"/>
+      <c r="D172" s="5"/>
+      <c r="E172" s="5"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A173" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B173" s="6"/>
+      <c r="C173" s="6"/>
+      <c r="D173" s="6"/>
+      <c r="E173" s="6"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A175" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A176" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A177" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A151:E152"/>
-    <mergeCell ref="A153:E153"/>
-    <mergeCell ref="A159:E160"/>
-    <mergeCell ref="A161:E161"/>
+  <mergeCells count="34">
+    <mergeCell ref="A160:E161"/>
+    <mergeCell ref="A162:E162"/>
     <mergeCell ref="A116:E117"/>
     <mergeCell ref="A118:E118"/>
     <mergeCell ref="A128:E129"/>
     <mergeCell ref="A130:E130"/>
-    <mergeCell ref="A143:E144"/>
-    <mergeCell ref="A145:E145"/>
-    <mergeCell ref="A81:E81"/>
-    <mergeCell ref="A87:E88"/>
+    <mergeCell ref="A144:E145"/>
+    <mergeCell ref="A146:E146"/>
     <mergeCell ref="A89:E89"/>
     <mergeCell ref="A108:E109"/>
     <mergeCell ref="A110:E110"/>
-    <mergeCell ref="A54:E54"/>
-    <mergeCell ref="A60:E61"/>
+    <mergeCell ref="A152:E153"/>
+    <mergeCell ref="A154:E154"/>
     <mergeCell ref="A62:E62"/>
     <mergeCell ref="A71:E72"/>
     <mergeCell ref="A73:E73"/>
+    <mergeCell ref="A81:E81"/>
+    <mergeCell ref="A87:E88"/>
+    <mergeCell ref="A171:E172"/>
+    <mergeCell ref="A173:E173"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A9:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A20:E21"/>
     <mergeCell ref="A79:E80"/>
     <mergeCell ref="A22:E22"/>
     <mergeCell ref="A30:E31"/>
@@ -2505,11 +2615,8 @@
     <mergeCell ref="A38:E39"/>
     <mergeCell ref="A40:E40"/>
     <mergeCell ref="A52:E53"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A9:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A20:E21"/>
+    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A60:E61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>